<commit_message>
minor in planif file
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/empty_planif_file.xlsx
+++ b/FlOpEDT/misc/deploy_database/empty_planif_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -189,6 +189,9 @@
       <t xml:space="preserve"> premiers cours de type « type » de la semaine</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve">(Ex : A3TD, A2CM, A1TP)</t>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -322,6 +325,12 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -469,7 +478,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -566,6 +575,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -645,8 +658,8 @@
   </sheetPr>
   <dimension ref="A1:DF9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="B24 E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2266,10 +2279,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2548,6 +2561,11 @@
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="24" t="s">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
new make planif File WITH RECAPgit add .
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/empty_planif_file.xlsx
+++ b/FlOpEDT/misc/deploy_database/empty_planif_file.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Règles" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Rules" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="empty_recap" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -29,6 +30,9 @@
     <t xml:space="preserve">Type de cours</t>
   </si>
   <si>
+    <t xml:space="preserve">Durée</t>
+  </si>
+  <si>
     <t xml:space="preserve">Prof</t>
   </si>
   <si>
@@ -39,6 +43,18 @@
   </si>
   <si>
     <t xml:space="preserve">TOTAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total heures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Semestre</t>
   </si>
   <si>
     <t xml:space="preserve">Mode de remplissage des colonnes du début</t>
@@ -189,6 +205,12 @@
   <si>
     <t xml:space="preserve">(Ex : A3TD, A2CM, A1TP)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Enseignant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSE</t>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +219,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -290,6 +312,34 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
@@ -323,8 +373,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,7 +416,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FFC5C5C5"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -381,12 +439,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFED1C24"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF37B70"/>
+        <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC5C5C5"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -437,6 +519,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thick"/>
       <right/>
       <top/>
@@ -469,7 +558,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -487,15 +576,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="6" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -539,35 +632,79 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -600,9 +737,9 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFF37B70"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -633,7 +770,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFED1C24"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -647,50 +784,52 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:DE9"/>
+  <dimension ref="A1:DG10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="6" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="27" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="32" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="53" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="58" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="79" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="104" min="84" style="0" width="4.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="109" min="105" style="0" width="2.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="995" min="110" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="996" style="0" width="11.34"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="2" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="8" style="0" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="29" style="0" width="2.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="34" style="0" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="55" style="0" width="2.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="60" style="0" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="81" style="0" width="2.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="86" style="0" width="4.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="107" style="0" width="2.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="997" min="112" style="0" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="998" style="0" width="11.34"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
@@ -793,15 +932,17 @@
       <c r="DC1" s="3"/>
       <c r="DD1" s="3"/>
       <c r="DE1" s="3"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="DF1" s="3"/>
+      <c r="DG1" s="3"/>
+    </row>
+    <row r="2" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
+      <c r="B2" s="4"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -904,666 +1045,703 @@
       <c r="DC2" s="6"/>
       <c r="DD2" s="6"/>
       <c r="DE2" s="6"/>
+      <c r="DF2" s="6"/>
+      <c r="DG2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="str">
+        <f aca="false">CONCATENATE($C3,"_",$E3)</f>
+        <v>_</v>
+      </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="7"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="10"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="10"/>
-      <c r="V3" s="10"/>
-      <c r="W3" s="10"/>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10"/>
-      <c r="Z3" s="10"/>
-      <c r="AA3" s="10"/>
-      <c r="AB3" s="10"/>
-      <c r="AC3" s="10"/>
-      <c r="AD3" s="10"/>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="10"/>
-      <c r="AG3" s="10"/>
-      <c r="AH3" s="10"/>
-      <c r="AI3" s="10"/>
-      <c r="AJ3" s="10"/>
-      <c r="AK3" s="10"/>
-      <c r="AL3" s="10"/>
-      <c r="AM3" s="10"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="10"/>
-      <c r="AP3" s="10"/>
-      <c r="AQ3" s="10"/>
-      <c r="AR3" s="10"/>
-      <c r="AS3" s="10"/>
-      <c r="AT3" s="10"/>
-      <c r="AU3" s="10"/>
-      <c r="AV3" s="10"/>
-      <c r="AW3" s="10"/>
-      <c r="AX3" s="10"/>
-      <c r="AY3" s="10"/>
-      <c r="AZ3" s="10"/>
-      <c r="BA3" s="10"/>
-      <c r="BB3" s="10"/>
-      <c r="BC3" s="10"/>
-      <c r="BD3" s="10"/>
-      <c r="BE3" s="10"/>
-      <c r="BF3" s="10"/>
-      <c r="BG3" s="10"/>
-      <c r="BH3" s="10"/>
-      <c r="BI3" s="10"/>
-      <c r="BJ3" s="10"/>
-      <c r="BK3" s="10"/>
-      <c r="BL3" s="10"/>
-      <c r="BM3" s="10"/>
-      <c r="BN3" s="10"/>
-      <c r="BO3" s="10"/>
-      <c r="BP3" s="10"/>
-      <c r="BQ3" s="10"/>
-      <c r="BR3" s="10"/>
-      <c r="BS3" s="10"/>
-      <c r="BT3" s="10"/>
-      <c r="BU3" s="10"/>
-      <c r="BV3" s="10"/>
-      <c r="BW3" s="10"/>
-      <c r="BX3" s="10"/>
-      <c r="BY3" s="10"/>
-      <c r="BZ3" s="10"/>
-      <c r="CA3" s="10"/>
-      <c r="CB3" s="10"/>
-      <c r="CC3" s="10"/>
-      <c r="CD3" s="10"/>
-      <c r="CE3" s="10"/>
-      <c r="CF3" s="10"/>
-      <c r="CG3" s="10"/>
-      <c r="CH3" s="10"/>
-      <c r="CI3" s="10"/>
-      <c r="CJ3" s="10"/>
-      <c r="CK3" s="10"/>
-      <c r="CL3" s="10"/>
-      <c r="CM3" s="10"/>
-      <c r="CN3" s="10"/>
-      <c r="CO3" s="10"/>
-      <c r="CP3" s="10"/>
-      <c r="CQ3" s="10"/>
-      <c r="CR3" s="10"/>
-      <c r="CS3" s="10"/>
-      <c r="CT3" s="10"/>
-      <c r="CU3" s="10"/>
-      <c r="CV3" s="10"/>
-      <c r="CW3" s="10"/>
-      <c r="CX3" s="10"/>
-      <c r="CY3" s="10"/>
-      <c r="CZ3" s="10"/>
-      <c r="DA3" s="10"/>
-      <c r="DB3" s="10"/>
-      <c r="DC3" s="10"/>
-      <c r="DD3" s="10"/>
-      <c r="DE3" s="10"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="11"/>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="11"/>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="11"/>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="11"/>
+      <c r="AW3" s="11"/>
+      <c r="AX3" s="11"/>
+      <c r="AY3" s="11"/>
+      <c r="AZ3" s="11"/>
+      <c r="BA3" s="11"/>
+      <c r="BB3" s="11"/>
+      <c r="BC3" s="11"/>
+      <c r="BD3" s="11"/>
+      <c r="BE3" s="11"/>
+      <c r="BF3" s="11"/>
+      <c r="BG3" s="11"/>
+      <c r="BH3" s="11"/>
+      <c r="BI3" s="11"/>
+      <c r="BJ3" s="11"/>
+      <c r="BK3" s="11"/>
+      <c r="BL3" s="11"/>
+      <c r="BM3" s="11"/>
+      <c r="BN3" s="11"/>
+      <c r="BO3" s="11"/>
+      <c r="BP3" s="11"/>
+      <c r="BQ3" s="11"/>
+      <c r="BR3" s="11"/>
+      <c r="BS3" s="11"/>
+      <c r="BT3" s="11"/>
+      <c r="BU3" s="11"/>
+      <c r="BV3" s="11"/>
+      <c r="BW3" s="11"/>
+      <c r="BX3" s="11"/>
+      <c r="BY3" s="11"/>
+      <c r="BZ3" s="11"/>
+      <c r="CA3" s="11"/>
+      <c r="CB3" s="11"/>
+      <c r="CC3" s="11"/>
+      <c r="CD3" s="11"/>
+      <c r="CE3" s="11"/>
+      <c r="CF3" s="11"/>
+      <c r="CG3" s="11"/>
+      <c r="CH3" s="11"/>
+      <c r="CI3" s="11"/>
+      <c r="CJ3" s="11"/>
+      <c r="CK3" s="11"/>
+      <c r="CL3" s="11"/>
+      <c r="CM3" s="11"/>
+      <c r="CN3" s="11"/>
+      <c r="CO3" s="11"/>
+      <c r="CP3" s="11"/>
+      <c r="CQ3" s="11"/>
+      <c r="CR3" s="11"/>
+      <c r="CS3" s="11"/>
+      <c r="CT3" s="11"/>
+      <c r="CU3" s="11"/>
+      <c r="CV3" s="11"/>
+      <c r="CW3" s="11"/>
+      <c r="CX3" s="11"/>
+      <c r="CY3" s="11"/>
+      <c r="CZ3" s="11"/>
+      <c r="DA3" s="11"/>
+      <c r="DB3" s="11"/>
+      <c r="DC3" s="11"/>
+      <c r="DD3" s="11"/>
+      <c r="DE3" s="11"/>
+      <c r="DF3" s="11"/>
+      <c r="DG3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="16"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16"/>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="16"/>
-      <c r="AB4" s="16"/>
-      <c r="AC4" s="16"/>
-      <c r="AD4" s="16"/>
-      <c r="AE4" s="16"/>
-      <c r="AF4" s="16"/>
-      <c r="AG4" s="16"/>
-      <c r="AH4" s="16"/>
-      <c r="AI4" s="16"/>
-      <c r="AJ4" s="16"/>
-      <c r="AK4" s="16"/>
-      <c r="AL4" s="16"/>
-      <c r="AM4" s="16"/>
-      <c r="AN4" s="16"/>
-      <c r="AO4" s="16"/>
-      <c r="AP4" s="16"/>
-      <c r="AQ4" s="16"/>
-      <c r="AR4" s="16"/>
-      <c r="AS4" s="16"/>
-      <c r="AT4" s="16"/>
-      <c r="AU4" s="16"/>
-      <c r="AV4" s="16"/>
-      <c r="AW4" s="16"/>
-      <c r="AX4" s="16"/>
-      <c r="AY4" s="16"/>
-      <c r="AZ4" s="16"/>
-      <c r="BA4" s="16"/>
-      <c r="BB4" s="16"/>
-      <c r="BC4" s="16"/>
-      <c r="BD4" s="16"/>
-      <c r="BE4" s="16"/>
-      <c r="BF4" s="16"/>
-      <c r="BG4" s="16"/>
-      <c r="BH4" s="16"/>
-      <c r="BI4" s="16"/>
-      <c r="BJ4" s="16"/>
-      <c r="BK4" s="16"/>
-      <c r="BL4" s="16"/>
-      <c r="BM4" s="16"/>
-      <c r="BN4" s="16"/>
-      <c r="BO4" s="16"/>
-      <c r="BP4" s="16"/>
-      <c r="BQ4" s="16"/>
-      <c r="BR4" s="16"/>
-      <c r="BS4" s="16"/>
-      <c r="BT4" s="16"/>
-      <c r="BU4" s="16"/>
-      <c r="BV4" s="16"/>
-      <c r="BW4" s="16"/>
-      <c r="BX4" s="16"/>
-      <c r="BY4" s="16"/>
-      <c r="BZ4" s="16"/>
-      <c r="CA4" s="16"/>
-      <c r="CB4" s="16"/>
-      <c r="CC4" s="16"/>
-      <c r="CD4" s="16"/>
-      <c r="CE4" s="16"/>
-      <c r="CF4" s="16"/>
-      <c r="CG4" s="16"/>
-      <c r="CH4" s="16"/>
-      <c r="CI4" s="16"/>
-      <c r="CJ4" s="16"/>
-      <c r="CK4" s="16"/>
-      <c r="CL4" s="16"/>
-      <c r="CM4" s="16"/>
-      <c r="CN4" s="16"/>
-      <c r="CO4" s="16"/>
-      <c r="CP4" s="16"/>
-      <c r="CQ4" s="16"/>
-      <c r="CR4" s="16"/>
-      <c r="CS4" s="16"/>
-      <c r="CT4" s="16"/>
-      <c r="CU4" s="16"/>
-      <c r="CV4" s="16"/>
-      <c r="CW4" s="16"/>
-      <c r="CX4" s="16"/>
-      <c r="CY4" s="16"/>
-      <c r="CZ4" s="16"/>
-      <c r="DA4" s="16"/>
-      <c r="DB4" s="16"/>
-      <c r="DC4" s="16"/>
-      <c r="DD4" s="16"/>
-      <c r="DE4" s="16"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",F$2:F$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",G$2:G$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",H$2:H$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",I$2:I$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",J$2:J$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",K$2:K$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="L5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",L$2:L$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="M5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",M$2:M$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="N5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",N$2:N$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="O5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",O$2:O$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",P$2:P$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Q5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",Q$2:Q$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",R$2:R$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="S5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",S$2:S$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="T5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",T$2:T$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="U5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",U$2:U$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",V$2:V$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="W5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",W$2:W$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="X5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",X$2:X$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",Y$2:Y$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",Z$2:Z$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AA$2:AA$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AB$2:AB$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AC$2:AC$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AD$2:AD$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AE$2:AE$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AF5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AF$2:AF$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AG5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AG$2:AG$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AH5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AH$2:AH$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AI5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AI$2:AI$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AJ$2:AJ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AK5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AK$2:AK$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AL5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AL$2:AL$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AM5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AM$2:AM$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AN5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AN$2:AN$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AO5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AO$2:AO$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AP5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AP$2:AP$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AQ$2:AQ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AR5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AR$2:AR$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AS5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AS$2:AS$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AT5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AT$2:AT$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AU5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AU$2:AU$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AV5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AV$2:AV$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AW5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AW$2:AW$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AX5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AX$2:AX$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AY5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AY$2:AY$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="AZ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",AZ$2:AZ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BA5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BA$2:BA$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BB5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BB$2:BB$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BC5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BC$2:BC$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BD5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BD$2:BD$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BE5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BE$2:BE$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BF5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BF$2:BF$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BG5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BG$2:BG$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BH5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BH$2:BH$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BI5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BI$2:BI$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BJ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BJ$2:BJ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BK5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BK$2:BK$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BL5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BL$2:BL$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BM5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BM$2:BM$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BN5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BN$2:BN$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BO5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BO$2:BO$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BP5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BP$2:BP$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BQ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BQ$2:BQ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BR5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BR$2:BR$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BS5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BS$2:BS$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BT5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BT$2:BT$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BU5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BU$2:BU$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BV5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BV$2:BV$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BW5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BW$2:BW$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BX5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BX$2:BX$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BY5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BY$2:BY$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="BZ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",BZ$2:BZ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CA5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CA$2:CA$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CB5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CB$2:CB$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CC5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CC$2:CC$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CD5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CD$2:CD$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CE5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CE$2:CE$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CF5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CF$2:CF$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CG5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CG$2:CG$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CH5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CH$2:CH$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CI5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CI$2:CI$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CJ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CJ$2:CJ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CK5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CK$2:CK$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CL5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CL$2:CL$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CM5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CM$2:CM$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CN5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CN$2:CN$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CO5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CO$2:CO$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CP5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CP$2:CP$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CQ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CQ$2:CQ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CR5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CR$2:CR$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CS5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CS$2:CS$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CT5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CT$2:CT$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CU5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CU$2:CU$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CV5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CV$2:CV$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CW5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CW$2:CW$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CX5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CX$2:CX$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CY5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CY$2:CY$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="CZ5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",CZ$2:CZ$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="DA5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",DA$2:DA$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="DB5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",DB$2:DB$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="DC5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",DC$2:DC$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="DD5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",DD$2:DD$4),0)</f>
-        <v>0</v>
-      </c>
-      <c r="DE5" s="18" t="n">
-        <f aca="false">ROUNDUP(SUMIF($D$2:$D$4,"",DE$2:DE$4),0)</f>
-        <v>0</v>
-      </c>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="17"/>
+      <c r="AC4" s="17"/>
+      <c r="AD4" s="17"/>
+      <c r="AE4" s="17"/>
+      <c r="AF4" s="17"/>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="17"/>
+      <c r="AJ4" s="17"/>
+      <c r="AK4" s="17"/>
+      <c r="AL4" s="17"/>
+      <c r="AM4" s="17"/>
+      <c r="AN4" s="17"/>
+      <c r="AO4" s="17"/>
+      <c r="AP4" s="17"/>
+      <c r="AQ4" s="17"/>
+      <c r="AR4" s="17"/>
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="17"/>
+      <c r="AU4" s="17"/>
+      <c r="AV4" s="17"/>
+      <c r="AW4" s="17"/>
+      <c r="AX4" s="17"/>
+      <c r="AY4" s="17"/>
+      <c r="AZ4" s="17"/>
+      <c r="BA4" s="17"/>
+      <c r="BB4" s="17"/>
+      <c r="BC4" s="17"/>
+      <c r="BD4" s="17"/>
+      <c r="BE4" s="17"/>
+      <c r="BF4" s="17"/>
+      <c r="BG4" s="17"/>
+      <c r="BH4" s="17"/>
+      <c r="BI4" s="17"/>
+      <c r="BJ4" s="17"/>
+      <c r="BK4" s="17"/>
+      <c r="BL4" s="17"/>
+      <c r="BM4" s="17"/>
+      <c r="BN4" s="17"/>
+      <c r="BO4" s="17"/>
+      <c r="BP4" s="17"/>
+      <c r="BQ4" s="17"/>
+      <c r="BR4" s="17"/>
+      <c r="BS4" s="17"/>
+      <c r="BT4" s="17"/>
+      <c r="BU4" s="17"/>
+      <c r="BV4" s="17"/>
+      <c r="BW4" s="17"/>
+      <c r="BX4" s="17"/>
+      <c r="BY4" s="17"/>
+      <c r="BZ4" s="17"/>
+      <c r="CA4" s="17"/>
+      <c r="CB4" s="17"/>
+      <c r="CC4" s="17"/>
+      <c r="CD4" s="17"/>
+      <c r="CE4" s="17"/>
+      <c r="CF4" s="17"/>
+      <c r="CG4" s="17"/>
+      <c r="CH4" s="17"/>
+      <c r="CI4" s="17"/>
+      <c r="CJ4" s="17"/>
+      <c r="CK4" s="17"/>
+      <c r="CL4" s="17"/>
+      <c r="CM4" s="17"/>
+      <c r="CN4" s="17"/>
+      <c r="CO4" s="17"/>
+      <c r="CP4" s="17"/>
+      <c r="CQ4" s="17"/>
+      <c r="CR4" s="17"/>
+      <c r="CS4" s="17"/>
+      <c r="CT4" s="17"/>
+      <c r="CU4" s="17"/>
+      <c r="CV4" s="17"/>
+      <c r="CW4" s="17"/>
+      <c r="CX4" s="17"/>
+      <c r="CY4" s="17"/>
+      <c r="CZ4" s="17"/>
+      <c r="DA4" s="17"/>
+      <c r="DB4" s="17"/>
+      <c r="DC4" s="17"/>
+      <c r="DD4" s="17"/>
+      <c r="DE4" s="17"/>
+      <c r="DF4" s="17"/>
+      <c r="DG4" s="17"/>
+    </row>
+    <row r="5" s="20" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
+      <c r="Q5" s="19"/>
+      <c r="R5" s="19"/>
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="19"/>
+      <c r="V5" s="19"/>
+      <c r="W5" s="19"/>
+      <c r="X5" s="19"/>
+      <c r="Y5" s="19"/>
+      <c r="Z5" s="19"/>
+      <c r="AA5" s="19"/>
+      <c r="AB5" s="19"/>
+      <c r="AC5" s="19"/>
+      <c r="AD5" s="19"/>
+      <c r="AE5" s="19"/>
+      <c r="AF5" s="19"/>
+      <c r="AG5" s="19"/>
+      <c r="AH5" s="19"/>
+      <c r="AI5" s="19"/>
+      <c r="AJ5" s="19"/>
+      <c r="AK5" s="19"/>
+      <c r="AL5" s="19"/>
+      <c r="AM5" s="19"/>
+      <c r="AN5" s="19"/>
+      <c r="AO5" s="19"/>
+      <c r="AP5" s="19"/>
+      <c r="AQ5" s="19"/>
+      <c r="AR5" s="19"/>
+      <c r="AS5" s="19"/>
+      <c r="AT5" s="19"/>
+      <c r="AU5" s="19"/>
+      <c r="AV5" s="19"/>
+      <c r="AW5" s="19"/>
+      <c r="AX5" s="19"/>
+      <c r="AY5" s="19"/>
+      <c r="AZ5" s="19"/>
+      <c r="BA5" s="19"/>
+      <c r="BB5" s="19"/>
+      <c r="BC5" s="19"/>
+      <c r="BD5" s="19"/>
+      <c r="BE5" s="19"/>
+      <c r="BF5" s="19"/>
+      <c r="BG5" s="19"/>
+      <c r="BH5" s="19"/>
+      <c r="BI5" s="19"/>
+      <c r="BJ5" s="19"/>
+      <c r="BK5" s="19"/>
+      <c r="BL5" s="19"/>
+      <c r="BM5" s="19"/>
+      <c r="BN5" s="19"/>
+      <c r="BO5" s="19"/>
+      <c r="BP5" s="19"/>
+      <c r="BQ5" s="19"/>
+      <c r="BR5" s="19"/>
+      <c r="BS5" s="19"/>
+      <c r="BT5" s="19"/>
+      <c r="BU5" s="19"/>
+      <c r="BV5" s="19"/>
+      <c r="BW5" s="19"/>
+      <c r="BX5" s="19"/>
+      <c r="BY5" s="19"/>
+      <c r="BZ5" s="19"/>
+      <c r="CA5" s="19"/>
+      <c r="CB5" s="19"/>
+      <c r="CC5" s="19"/>
+      <c r="CD5" s="19"/>
+      <c r="CE5" s="19"/>
+      <c r="CF5" s="19"/>
+      <c r="CG5" s="19"/>
+      <c r="CH5" s="19"/>
+      <c r="CI5" s="19"/>
+      <c r="CJ5" s="19"/>
+      <c r="CK5" s="19"/>
+      <c r="CL5" s="19"/>
+      <c r="CM5" s="19"/>
+      <c r="CN5" s="19"/>
+      <c r="CO5" s="19"/>
+      <c r="CP5" s="19"/>
+      <c r="CQ5" s="19"/>
+      <c r="CR5" s="19"/>
+      <c r="CS5" s="19"/>
+      <c r="CT5" s="19"/>
+      <c r="CU5" s="19"/>
+      <c r="CV5" s="19"/>
+      <c r="CW5" s="19"/>
+      <c r="CX5" s="19"/>
+      <c r="CY5" s="19"/>
+      <c r="CZ5" s="19"/>
+      <c r="DA5" s="19"/>
+      <c r="DB5" s="19"/>
+      <c r="DC5" s="19"/>
+      <c r="DD5" s="19"/>
+      <c r="DE5" s="19"/>
+      <c r="DF5" s="19"/>
+      <c r="DG5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+      <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AS7" s="3"/>
+      <c r="AT7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AV7" s="3"/>
+      <c r="AW7" s="3"/>
+      <c r="AX7" s="3"/>
+      <c r="AY7" s="3"/>
+      <c r="AZ7" s="3"/>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="3"/>
+      <c r="BK7" s="3"/>
+      <c r="BL7" s="3"/>
+      <c r="BM7" s="3"/>
+      <c r="BN7" s="3"/>
+      <c r="BO7" s="3"/>
+      <c r="BP7" s="3"/>
+      <c r="BQ7" s="3"/>
+      <c r="BR7" s="3"/>
+      <c r="BS7" s="3"/>
+      <c r="BT7" s="3"/>
+      <c r="BU7" s="3"/>
+      <c r="BV7" s="3"/>
+      <c r="BW7" s="3"/>
+      <c r="BX7" s="3"/>
+      <c r="BY7" s="3"/>
+      <c r="BZ7" s="3"/>
+      <c r="CA7" s="3"/>
+      <c r="CB7" s="3"/>
+      <c r="CC7" s="3"/>
+      <c r="CD7" s="3"/>
+      <c r="CE7" s="3"/>
+      <c r="CF7" s="3"/>
+      <c r="CG7" s="3"/>
+      <c r="CH7" s="3"/>
+      <c r="CI7" s="3"/>
+      <c r="CJ7" s="3"/>
+      <c r="CK7" s="3"/>
+      <c r="CL7" s="3"/>
+      <c r="CM7" s="3"/>
+      <c r="CN7" s="3"/>
+      <c r="CO7" s="3"/>
+      <c r="CP7" s="3"/>
+      <c r="CQ7" s="3"/>
+      <c r="CR7" s="3"/>
+      <c r="CS7" s="3"/>
+      <c r="CT7" s="3"/>
+      <c r="CU7" s="3"/>
+      <c r="CV7" s="3"/>
+      <c r="CW7" s="3"/>
+      <c r="CX7" s="3"/>
+      <c r="CY7" s="3"/>
+      <c r="CZ7" s="3"/>
+      <c r="DA7" s="3"/>
+      <c r="DB7" s="3"/>
+      <c r="DC7" s="3"/>
+      <c r="DD7" s="3"/>
+      <c r="DE7" s="3"/>
+      <c r="DF7" s="3"/>
+      <c r="DG7" s="3"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E8" s="24"/>
+      <c r="F8" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="27"/>
+      <c r="I8" s="27"/>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+      <c r="P8" s="27"/>
+      <c r="Q8" s="27"/>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27"/>
+      <c r="U8" s="27"/>
+      <c r="V8" s="27"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="27"/>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AB8" s="27"/>
+      <c r="AC8" s="27"/>
+      <c r="AD8" s="27"/>
+      <c r="AE8" s="27"/>
+      <c r="AF8" s="27"/>
+      <c r="AG8" s="27"/>
+      <c r="AH8" s="27"/>
+      <c r="AI8" s="27"/>
+      <c r="AJ8" s="27"/>
+      <c r="AK8" s="27"/>
+      <c r="AL8" s="27"/>
+      <c r="AM8" s="27"/>
+      <c r="AN8" s="27"/>
+      <c r="AO8" s="27"/>
+      <c r="AP8" s="27"/>
+      <c r="AQ8" s="27"/>
+      <c r="AR8" s="27"/>
+      <c r="AS8" s="27"/>
+      <c r="AT8" s="27"/>
+      <c r="AU8" s="27"/>
+      <c r="AV8" s="27"/>
+      <c r="AW8" s="27"/>
+      <c r="AX8" s="27"/>
+      <c r="AY8" s="27"/>
+      <c r="AZ8" s="27"/>
+      <c r="BA8" s="27"/>
+      <c r="BB8" s="27"/>
+      <c r="BC8" s="27"/>
+      <c r="BD8" s="27"/>
+      <c r="BE8" s="27"/>
+      <c r="BF8" s="27"/>
+      <c r="BG8" s="27"/>
+      <c r="BH8" s="27"/>
+      <c r="BI8" s="27"/>
+      <c r="BJ8" s="27"/>
+      <c r="BK8" s="27"/>
+      <c r="BL8" s="27"/>
+      <c r="BM8" s="27"/>
+      <c r="BN8" s="27"/>
+      <c r="BO8" s="27"/>
+      <c r="BP8" s="27"/>
+      <c r="BQ8" s="27"/>
+      <c r="BR8" s="27"/>
+      <c r="BS8" s="27"/>
+      <c r="BT8" s="27"/>
+      <c r="BU8" s="27"/>
+      <c r="BV8" s="27"/>
+      <c r="BW8" s="27"/>
+      <c r="BX8" s="27"/>
+      <c r="BY8" s="27"/>
+      <c r="BZ8" s="27"/>
+      <c r="CA8" s="27"/>
+      <c r="CB8" s="27"/>
+      <c r="CC8" s="27"/>
+      <c r="CD8" s="27"/>
+      <c r="CE8" s="27"/>
+      <c r="CF8" s="27"/>
+      <c r="CG8" s="27"/>
+      <c r="CH8" s="27"/>
+      <c r="CI8" s="27"/>
+      <c r="CJ8" s="27"/>
+      <c r="CK8" s="27"/>
+      <c r="CL8" s="27"/>
+      <c r="CM8" s="27"/>
+      <c r="CN8" s="27"/>
+      <c r="CO8" s="27"/>
+      <c r="CP8" s="27"/>
+      <c r="CQ8" s="27"/>
+      <c r="CR8" s="27"/>
+      <c r="CS8" s="27"/>
+      <c r="CT8" s="27"/>
+      <c r="CU8" s="27"/>
+      <c r="CV8" s="27"/>
+      <c r="CW8" s="27"/>
+      <c r="CX8" s="27"/>
+      <c r="CY8" s="27"/>
+      <c r="CZ8" s="27"/>
+      <c r="DA8" s="27"/>
+      <c r="DB8" s="27"/>
+      <c r="DC8" s="27"/>
+      <c r="DD8" s="27"/>
+      <c r="DE8" s="27"/>
+      <c r="DF8" s="27"/>
+      <c r="DG8" s="27"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E9" s="24"/>
+      <c r="F9" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="28"/>
+      <c r="P9" s="28"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="W9" s="28"/>
+      <c r="X9" s="28"/>
+      <c r="Y9" s="28"/>
+      <c r="Z9" s="28"/>
+      <c r="AA9" s="28"/>
+      <c r="AB9" s="28"/>
+      <c r="AC9" s="28"/>
+      <c r="AD9" s="28"/>
+      <c r="AE9" s="28"/>
+      <c r="AF9" s="28"/>
+      <c r="AG9" s="28"/>
+      <c r="AH9" s="28"/>
+      <c r="AI9" s="28"/>
+      <c r="AJ9" s="28"/>
+      <c r="AK9" s="28"/>
+      <c r="AL9" s="28"/>
+      <c r="AM9" s="28"/>
+      <c r="AN9" s="28"/>
+      <c r="AO9" s="28"/>
+      <c r="AP9" s="28"/>
+      <c r="AQ9" s="28"/>
+      <c r="AR9" s="28"/>
+      <c r="AS9" s="28"/>
+      <c r="AT9" s="28"/>
+      <c r="AU9" s="28"/>
+      <c r="AV9" s="28"/>
+      <c r="AW9" s="28"/>
+      <c r="AX9" s="28"/>
+      <c r="AY9" s="28"/>
+      <c r="AZ9" s="28"/>
+      <c r="BA9" s="28"/>
+      <c r="BB9" s="28"/>
+      <c r="BC9" s="28"/>
+      <c r="BD9" s="28"/>
+      <c r="BE9" s="28"/>
+      <c r="BF9" s="28"/>
+      <c r="BG9" s="28"/>
+      <c r="BH9" s="28"/>
+      <c r="BI9" s="28"/>
+      <c r="BJ9" s="28"/>
+      <c r="BK9" s="28"/>
+      <c r="BL9" s="28"/>
+      <c r="BM9" s="28"/>
+      <c r="BN9" s="28"/>
+      <c r="BO9" s="28"/>
+      <c r="BP9" s="28"/>
+      <c r="BQ9" s="28"/>
+      <c r="BR9" s="28"/>
+      <c r="BS9" s="28"/>
+      <c r="BT9" s="28"/>
+      <c r="BU9" s="28"/>
+      <c r="BV9" s="28"/>
+      <c r="BW9" s="28"/>
+      <c r="BX9" s="28"/>
+      <c r="BY9" s="28"/>
+      <c r="BZ9" s="28"/>
+      <c r="CA9" s="28"/>
+      <c r="CB9" s="28"/>
+      <c r="CC9" s="28"/>
+      <c r="CD9" s="28"/>
+      <c r="CE9" s="28"/>
+      <c r="CF9" s="28"/>
+      <c r="CG9" s="28"/>
+      <c r="CH9" s="28"/>
+      <c r="CI9" s="28"/>
+      <c r="CJ9" s="28"/>
+      <c r="CK9" s="28"/>
+      <c r="CL9" s="28"/>
+      <c r="CM9" s="28"/>
+      <c r="CN9" s="28"/>
+      <c r="CO9" s="28"/>
+      <c r="CP9" s="28"/>
+      <c r="CQ9" s="28"/>
+      <c r="CR9" s="28"/>
+      <c r="CS9" s="28"/>
+      <c r="CT9" s="28"/>
+      <c r="CU9" s="28"/>
+      <c r="CV9" s="28"/>
+      <c r="CW9" s="28"/>
+      <c r="CX9" s="28"/>
+      <c r="CY9" s="28"/>
+      <c r="CZ9" s="28"/>
+      <c r="DA9" s="28"/>
+      <c r="DB9" s="28"/>
+      <c r="DC9" s="28"/>
+      <c r="DD9" s="28"/>
+      <c r="DE9" s="28"/>
+      <c r="DF9" s="28"/>
+      <c r="DG9" s="28"/>
+    </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2243,7 +2421,6 @@
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="689" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2262,8 +2439,8 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2274,286 +2451,704 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30"/>
+      <c r="B5" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="30"/>
+      <c r="B11" s="33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="30"/>
+      <c r="B13" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="30"/>
+      <c r="B14" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="31"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="30"/>
+      <c r="B22" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AV3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="3" style="0" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="21" style="0" width="2.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="3.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="32" style="0" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="49" style="0" width="4.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="72" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="E1" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="K1" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="L1" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="M1" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="N1" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="O1" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="P1" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="R1" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="S1" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="T1" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="U1" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="V1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W1" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="X1" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="AA1" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="21" t="s">
+      <c r="AB1" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="20"/>
-      <c r="B5" s="23" t="s">
+      <c r="AC1" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20" t="s">
+      <c r="AD1" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="AE1" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="23" t="s">
+      <c r="AF1" s="3" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
+      <c r="AG1" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
+      <c r="AH1" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="AI1" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="20"/>
-      <c r="B11" s="23" t="s">
+      <c r="AJ1" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20" t="s">
+      <c r="AK1" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="AL1" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
-      <c r="B13" s="23" t="s">
+      <c r="AM1" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="20"/>
-      <c r="B14" s="23" t="s">
+      <c r="AN1" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="21"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19" t="s">
+      <c r="AO1" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="20" t="s">
+      <c r="AP1" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="AQ1" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="20" t="s">
+      <c r="AR1" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="AS1" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="20" t="s">
+      <c r="AT1" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="AU1" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21" t="s">
+      <c r="AV1" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="22"/>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="24" t="s">
-        <v>32</v>
-      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AG2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AK2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AL2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AM2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AN2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AP2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AR2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AT2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AU2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AV2" s="27" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="36"/>
+      <c r="AE3" s="36"/>
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" s="36"/>
+      <c r="AJ3" s="36"/>
+      <c r="AK3" s="36"/>
+      <c r="AL3" s="36"/>
+      <c r="AM3" s="36"/>
+      <c r="AN3" s="36"/>
+      <c r="AO3" s="36"/>
+      <c r="AP3" s="36"/>
+      <c r="AQ3" s="36"/>
+      <c r="AR3" s="36"/>
+      <c r="AS3" s="36"/>
+      <c r="AT3" s="36"/>
+      <c r="AU3" s="36"/>
+      <c r="AV3" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A17:I17"/>
-  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Final modifications on planif file
</commit_message>
<xml_diff>
--- a/FlOpEDT/misc/deploy_database/empty_planif_file.xlsx
+++ b/FlOpEDT/misc/deploy_database/empty_planif_file.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="empty" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t xml:space="preserve">Module</t>
   </si>
@@ -45,10 +45,7 @@
     <t xml:space="preserve">TOTAL</t>
   </si>
   <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total heures</t>
+    <t xml:space="preserve">Heures</t>
   </si>
   <si>
     <t xml:space="preserve">type</t>
@@ -209,7 +206,7 @@
     <t xml:space="preserve">Enseignant</t>
   </si>
   <si>
-    <t xml:space="preserve">PSE</t>
+    <t xml:space="preserve">TEST</t>
   </si>
 </sst>
 </file>
@@ -445,12 +442,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF37B70"/>
-        <bgColor rgb="FFFF99CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
@@ -465,6 +456,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFC5C5C5"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF37B70"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -647,10 +644,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="11" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="9" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -659,23 +652,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="12" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,6 +690,10 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="14" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -784,10 +781,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:DG10"/>
+  <dimension ref="A1:DG9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5:F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1278,12 +1275,12 @@
       <c r="DG4" s="17"/>
     </row>
     <row r="5" s="20" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="A5" s="0"/>
+      <c r="B5" s="0"/>
+      <c r="C5" s="0"/>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="F5" s="0"/>
       <c r="G5" s="18" t="s">
         <v>6</v>
       </c>
@@ -1393,128 +1390,235 @@
       <c r="DG5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F6" s="21" t="s">
+      <c r="B6" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="22"/>
-    </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F7" s="23" t="s">
+      <c r="F6" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AS6" s="3"/>
+      <c r="AT6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AV6" s="3"/>
+      <c r="AW6" s="3"/>
+      <c r="AX6" s="3"/>
+      <c r="AY6" s="3"/>
+      <c r="AZ6" s="3"/>
+      <c r="BA6" s="3"/>
+      <c r="BB6" s="3"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
+      <c r="BI6" s="3"/>
+      <c r="BJ6" s="3"/>
+      <c r="BK6" s="3"/>
+      <c r="BL6" s="3"/>
+      <c r="BM6" s="3"/>
+      <c r="BN6" s="3"/>
+      <c r="BO6" s="3"/>
+      <c r="BP6" s="3"/>
+      <c r="BQ6" s="3"/>
+      <c r="BR6" s="3"/>
+      <c r="BS6" s="3"/>
+      <c r="BT6" s="3"/>
+      <c r="BU6" s="3"/>
+      <c r="BV6" s="3"/>
+      <c r="BW6" s="3"/>
+      <c r="BX6" s="3"/>
+      <c r="BY6" s="3"/>
+      <c r="BZ6" s="3"/>
+      <c r="CA6" s="3"/>
+      <c r="CB6" s="3"/>
+      <c r="CC6" s="3"/>
+      <c r="CD6" s="3"/>
+      <c r="CE6" s="3"/>
+      <c r="CF6" s="3"/>
+      <c r="CG6" s="3"/>
+      <c r="CH6" s="3"/>
+      <c r="CI6" s="3"/>
+      <c r="CJ6" s="3"/>
+      <c r="CK6" s="3"/>
+      <c r="CL6" s="3"/>
+      <c r="CM6" s="3"/>
+      <c r="CN6" s="3"/>
+      <c r="CO6" s="3"/>
+      <c r="CP6" s="3"/>
+      <c r="CQ6" s="3"/>
+      <c r="CR6" s="3"/>
+      <c r="CS6" s="3"/>
+      <c r="CT6" s="3"/>
+      <c r="CU6" s="3"/>
+      <c r="CV6" s="3"/>
+      <c r="CW6" s="3"/>
+      <c r="CX6" s="3"/>
+      <c r="CY6" s="3"/>
+      <c r="CZ6" s="3"/>
+      <c r="DA6" s="3"/>
+      <c r="DB6" s="3"/>
+      <c r="DC6" s="3"/>
+      <c r="DD6" s="3"/>
+      <c r="DE6" s="3"/>
+      <c r="DF6" s="3"/>
+      <c r="DG6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F7" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="3"/>
-      <c r="AQ7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
-      <c r="AU7" s="3"/>
-      <c r="AV7" s="3"/>
-      <c r="AW7" s="3"/>
-      <c r="AX7" s="3"/>
-      <c r="AY7" s="3"/>
-      <c r="AZ7" s="3"/>
-      <c r="BA7" s="3"/>
-      <c r="BB7" s="3"/>
-      <c r="BC7" s="3"/>
-      <c r="BD7" s="3"/>
-      <c r="BE7" s="3"/>
-      <c r="BF7" s="3"/>
-      <c r="BG7" s="3"/>
-      <c r="BH7" s="3"/>
-      <c r="BI7" s="3"/>
-      <c r="BJ7" s="3"/>
-      <c r="BK7" s="3"/>
-      <c r="BL7" s="3"/>
-      <c r="BM7" s="3"/>
-      <c r="BN7" s="3"/>
-      <c r="BO7" s="3"/>
-      <c r="BP7" s="3"/>
-      <c r="BQ7" s="3"/>
-      <c r="BR7" s="3"/>
-      <c r="BS7" s="3"/>
-      <c r="BT7" s="3"/>
-      <c r="BU7" s="3"/>
-      <c r="BV7" s="3"/>
-      <c r="BW7" s="3"/>
-      <c r="BX7" s="3"/>
-      <c r="BY7" s="3"/>
-      <c r="BZ7" s="3"/>
-      <c r="CA7" s="3"/>
-      <c r="CB7" s="3"/>
-      <c r="CC7" s="3"/>
-      <c r="CD7" s="3"/>
-      <c r="CE7" s="3"/>
-      <c r="CF7" s="3"/>
-      <c r="CG7" s="3"/>
-      <c r="CH7" s="3"/>
-      <c r="CI7" s="3"/>
-      <c r="CJ7" s="3"/>
-      <c r="CK7" s="3"/>
-      <c r="CL7" s="3"/>
-      <c r="CM7" s="3"/>
-      <c r="CN7" s="3"/>
-      <c r="CO7" s="3"/>
-      <c r="CP7" s="3"/>
-      <c r="CQ7" s="3"/>
-      <c r="CR7" s="3"/>
-      <c r="CS7" s="3"/>
-      <c r="CT7" s="3"/>
-      <c r="CU7" s="3"/>
-      <c r="CV7" s="3"/>
-      <c r="CW7" s="3"/>
-      <c r="CX7" s="3"/>
-      <c r="CY7" s="3"/>
-      <c r="CZ7" s="3"/>
-      <c r="DA7" s="3"/>
-      <c r="DB7" s="3"/>
-      <c r="DC7" s="3"/>
-      <c r="DD7" s="3"/>
-      <c r="DE7" s="3"/>
-      <c r="DF7" s="3"/>
-      <c r="DG7" s="3"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="26"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="26"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="26"/>
+      <c r="AA7" s="26"/>
+      <c r="AB7" s="26"/>
+      <c r="AC7" s="26"/>
+      <c r="AD7" s="26"/>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
+      <c r="AH7" s="26"/>
+      <c r="AI7" s="26"/>
+      <c r="AJ7" s="26"/>
+      <c r="AK7" s="26"/>
+      <c r="AL7" s="26"/>
+      <c r="AM7" s="26"/>
+      <c r="AN7" s="26"/>
+      <c r="AO7" s="26"/>
+      <c r="AP7" s="26"/>
+      <c r="AQ7" s="26"/>
+      <c r="AR7" s="26"/>
+      <c r="AS7" s="26"/>
+      <c r="AT7" s="26"/>
+      <c r="AU7" s="26"/>
+      <c r="AV7" s="26"/>
+      <c r="AW7" s="26"/>
+      <c r="AX7" s="26"/>
+      <c r="AY7" s="26"/>
+      <c r="AZ7" s="26"/>
+      <c r="BA7" s="26"/>
+      <c r="BB7" s="26"/>
+      <c r="BC7" s="26"/>
+      <c r="BD7" s="26"/>
+      <c r="BE7" s="26"/>
+      <c r="BF7" s="26"/>
+      <c r="BG7" s="26"/>
+      <c r="BH7" s="26"/>
+      <c r="BI7" s="26"/>
+      <c r="BJ7" s="26"/>
+      <c r="BK7" s="26"/>
+      <c r="BL7" s="26"/>
+      <c r="BM7" s="26"/>
+      <c r="BN7" s="26"/>
+      <c r="BO7" s="26"/>
+      <c r="BP7" s="26"/>
+      <c r="BQ7" s="26"/>
+      <c r="BR7" s="26"/>
+      <c r="BS7" s="26"/>
+      <c r="BT7" s="26"/>
+      <c r="BU7" s="26"/>
+      <c r="BV7" s="26"/>
+      <c r="BW7" s="26"/>
+      <c r="BX7" s="26"/>
+      <c r="BY7" s="26"/>
+      <c r="BZ7" s="26"/>
+      <c r="CA7" s="26"/>
+      <c r="CB7" s="26"/>
+      <c r="CC7" s="26"/>
+      <c r="CD7" s="26"/>
+      <c r="CE7" s="26"/>
+      <c r="CF7" s="26"/>
+      <c r="CG7" s="26"/>
+      <c r="CH7" s="26"/>
+      <c r="CI7" s="26"/>
+      <c r="CJ7" s="26"/>
+      <c r="CK7" s="26"/>
+      <c r="CL7" s="26"/>
+      <c r="CM7" s="26"/>
+      <c r="CN7" s="26"/>
+      <c r="CO7" s="26"/>
+      <c r="CP7" s="26"/>
+      <c r="CQ7" s="26"/>
+      <c r="CR7" s="26"/>
+      <c r="CS7" s="26"/>
+      <c r="CT7" s="26"/>
+      <c r="CU7" s="26"/>
+      <c r="CV7" s="26"/>
+      <c r="CW7" s="26"/>
+      <c r="CX7" s="26"/>
+      <c r="CY7" s="26"/>
+      <c r="CZ7" s="26"/>
+      <c r="DA7" s="26"/>
+      <c r="DB7" s="26"/>
+      <c r="DC7" s="26"/>
+      <c r="DD7" s="26"/>
+      <c r="DE7" s="26"/>
+      <c r="DF7" s="26"/>
+      <c r="DG7" s="26"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="26"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
@@ -1620,116 +1724,7 @@
       <c r="DF8" s="27"/>
       <c r="DG8" s="27"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F9" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
-      <c r="Z9" s="28"/>
-      <c r="AA9" s="28"/>
-      <c r="AB9" s="28"/>
-      <c r="AC9" s="28"/>
-      <c r="AD9" s="28"/>
-      <c r="AE9" s="28"/>
-      <c r="AF9" s="28"/>
-      <c r="AG9" s="28"/>
-      <c r="AH9" s="28"/>
-      <c r="AI9" s="28"/>
-      <c r="AJ9" s="28"/>
-      <c r="AK9" s="28"/>
-      <c r="AL9" s="28"/>
-      <c r="AM9" s="28"/>
-      <c r="AN9" s="28"/>
-      <c r="AO9" s="28"/>
-      <c r="AP9" s="28"/>
-      <c r="AQ9" s="28"/>
-      <c r="AR9" s="28"/>
-      <c r="AS9" s="28"/>
-      <c r="AT9" s="28"/>
-      <c r="AU9" s="28"/>
-      <c r="AV9" s="28"/>
-      <c r="AW9" s="28"/>
-      <c r="AX9" s="28"/>
-      <c r="AY9" s="28"/>
-      <c r="AZ9" s="28"/>
-      <c r="BA9" s="28"/>
-      <c r="BB9" s="28"/>
-      <c r="BC9" s="28"/>
-      <c r="BD9" s="28"/>
-      <c r="BE9" s="28"/>
-      <c r="BF9" s="28"/>
-      <c r="BG9" s="28"/>
-      <c r="BH9" s="28"/>
-      <c r="BI9" s="28"/>
-      <c r="BJ9" s="28"/>
-      <c r="BK9" s="28"/>
-      <c r="BL9" s="28"/>
-      <c r="BM9" s="28"/>
-      <c r="BN9" s="28"/>
-      <c r="BO9" s="28"/>
-      <c r="BP9" s="28"/>
-      <c r="BQ9" s="28"/>
-      <c r="BR9" s="28"/>
-      <c r="BS9" s="28"/>
-      <c r="BT9" s="28"/>
-      <c r="BU9" s="28"/>
-      <c r="BV9" s="28"/>
-      <c r="BW9" s="28"/>
-      <c r="BX9" s="28"/>
-      <c r="BY9" s="28"/>
-      <c r="BZ9" s="28"/>
-      <c r="CA9" s="28"/>
-      <c r="CB9" s="28"/>
-      <c r="CC9" s="28"/>
-      <c r="CD9" s="28"/>
-      <c r="CE9" s="28"/>
-      <c r="CF9" s="28"/>
-      <c r="CG9" s="28"/>
-      <c r="CH9" s="28"/>
-      <c r="CI9" s="28"/>
-      <c r="CJ9" s="28"/>
-      <c r="CK9" s="28"/>
-      <c r="CL9" s="28"/>
-      <c r="CM9" s="28"/>
-      <c r="CN9" s="28"/>
-      <c r="CO9" s="28"/>
-      <c r="CP9" s="28"/>
-      <c r="CQ9" s="28"/>
-      <c r="CR9" s="28"/>
-      <c r="CS9" s="28"/>
-      <c r="CT9" s="28"/>
-      <c r="CU9" s="28"/>
-      <c r="CV9" s="28"/>
-      <c r="CW9" s="28"/>
-      <c r="CX9" s="28"/>
-      <c r="CY9" s="28"/>
-      <c r="CZ9" s="28"/>
-      <c r="DA9" s="28"/>
-      <c r="DB9" s="28"/>
-      <c r="DC9" s="28"/>
-      <c r="DD9" s="28"/>
-      <c r="DE9" s="28"/>
-      <c r="DF9" s="28"/>
-      <c r="DG9" s="28"/>
-    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2408,7 +2403,6 @@
     <row r="685" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="686" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="687" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="688" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2428,7 +2422,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="1" sqref="A5:F5 A17"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2439,278 +2433,278 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="31" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="30"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="31" t="s">
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="29"/>
+      <c r="B5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30"/>
-      <c r="B5" s="33" t="s">
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="30" t="s">
+      <c r="B6" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="32"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="33" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="28" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="30" t="s">
+      <c r="B10" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="29"/>
+      <c r="B11" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="30"/>
-      <c r="B11" s="33" t="s">
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="30" t="s">
+      <c r="B12" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="29"/>
+      <c r="B13" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="30"/>
-      <c r="B13" s="33" t="s">
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="29"/>
+      <c r="B14" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="32"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="30"/>
-      <c r="B14" s="33" t="s">
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="30"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="32"/>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="31"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29" t="s">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
-      <c r="E17" s="29"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="29"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="30" t="s">
+      <c r="B18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="30" t="s">
+      <c r="B19" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="30" t="s">
+      <c r="B20" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="29"/>
+      <c r="B21" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="32"/>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
-      <c r="I20" s="32"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31" t="s">
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="29"/>
+      <c r="B22" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31" t="s">
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="31"/>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="30" t="s">
+      <c r="B23" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="31" t="s">
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="33" t="s">
         <v>36</v>
-      </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="32"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="34" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2731,8 +2725,8 @@
   </sheetPr>
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A5:F5 B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q6" activeCellId="0" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2750,10 +2744,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="34" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>39</v>
       </c>
       <c r="C1" s="3" t="n">
         <v>35</v>
@@ -2895,191 +2889,191 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="D2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="H2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="I2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="J2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="K2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="L2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="M2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="N2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="O2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="P2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="Q2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="R2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="S2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="T2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="U2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="V2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="W2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="X2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="Y2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="Z2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AA2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AB2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AC2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AD2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AE2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AF2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AG2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AH2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AI2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AK2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AL2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AM2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AN2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AO2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AP2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AR2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AS2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AT2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AU2" s="27" t="n">
-        <f aca="false">0</f>
-        <v>0</v>
-      </c>
-      <c r="AV2" s="27" t="n">
+      <c r="A2" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AC2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AD2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AF2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AG2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AI2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AK2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AL2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AM2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AN2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AO2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AP2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AR2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AS2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AT2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AU2" s="26" t="n">
+        <f aca="false">0</f>
+        <v>0</v>
+      </c>
+      <c r="AV2" s="26" t="n">
         <f aca="false">0</f>
         <v>0</v>
       </c>

</xml_diff>